<commit_message>
Cambios finales en documentación para entrega
</commit_message>
<xml_diff>
--- a/Editables/cronograma.xlsx
+++ b/Editables/cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Descargas\Octavo Semestre\Computacion Grafica\ProyFinal\ProyectoCG\Editables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilia\Desktop\Proyecto_CG\Editables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3B435F-0E49-458A-9574-4C3589334AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DDDF3A-47CB-4D69-A4A9-A1AABECAAA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A81C6D7D-8F9D-47F5-B466-7877C279A443}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A81C6D7D-8F9D-47F5-B466-7877C279A443}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -687,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6E7E03-6D1C-4CA1-87FF-7067265402C9}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1159,7 +1159,7 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:M2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.94488188976377963" right="0.94488188976377963" top="0.94488188976377963" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se modfican archivos de configuracion
</commit_message>
<xml_diff>
--- a/Editables/cronograma.xlsx
+++ b/Editables/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kilia\Desktop\Proyecto_CG\Editables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DDDF3A-47CB-4D69-A4A9-A1AABECAAA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C891F4-2A7E-4EBD-998A-AD3F2E9062D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A81C6D7D-8F9D-47F5-B466-7877C279A443}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="26">
   <si>
     <t>Cronograma de actividades</t>
   </si>
@@ -104,6 +104,15 @@
   </si>
   <si>
     <t>Todo el equipo</t>
+  </si>
+  <si>
+    <t>Adición de luces</t>
+  </si>
+  <si>
+    <t>Incorporación de cámaras</t>
+  </si>
+  <si>
+    <t>Valencia</t>
   </si>
 </sst>
 </file>
@@ -159,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -249,11 +258,93 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -264,7 +355,9 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -274,8 +367,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -285,8 +382,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -296,15 +397,64 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,28 +468,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -348,13 +549,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -685,10 +886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6E7E03-6D1C-4CA1-87FF-7067265402C9}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,152 +898,240 @@
     <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="12" width="3.77734375" customWidth="1"/>
-    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="27" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:27" s="30" customFormat="1" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="20"/>
-    </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="10">
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="37"/>
+    </row>
+    <row r="3" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="8">
         <v>4</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>5</v>
       </c>
-      <c r="G3" s="11">
-        <v>6</v>
-      </c>
-      <c r="H3" s="11">
+      <c r="G3" s="9">
+        <v>6</v>
+      </c>
+      <c r="H3" s="9">
         <v>7</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="9">
         <v>8</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="9">
         <v>9</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="9">
         <v>10</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="9">
         <v>11</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="10">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="N3" s="9">
+        <v>13</v>
+      </c>
+      <c r="O3" s="9">
+        <v>14</v>
+      </c>
+      <c r="P3" s="9">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>16</v>
+      </c>
+      <c r="R3" s="9">
+        <v>17</v>
+      </c>
+      <c r="S3" s="9">
+        <v>18</v>
+      </c>
+      <c r="T3" s="9">
+        <v>19</v>
+      </c>
+      <c r="U3" s="9">
+        <v>20</v>
+      </c>
+      <c r="V3" s="9">
+        <v>21</v>
+      </c>
+      <c r="W3" s="9">
+        <v>22</v>
+      </c>
+      <c r="X3" s="9">
+        <v>23</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>24</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="11">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="14">
         <v>44685</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="15">
         <v>44686</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="E4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="24"/>
+    </row>
+    <row r="5" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>44685</v>
       </c>
-      <c r="D5" s="6">
-        <v>44692</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="8" t="s">
+      <c r="D5" s="17">
+        <v>44703</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="18"/>
+    </row>
+    <row r="6" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>44685</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="17">
         <v>44685</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="26" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4"/>
@@ -853,265 +1142,441 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="18"/>
+    </row>
+    <row r="7" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>44685</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="17">
         <v>44692</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="8" t="s">
+      <c r="E7" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="18"/>
+    </row>
+    <row r="8" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>44691</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="17">
         <v>44692</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="8" t="s">
+      <c r="K8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="18"/>
+    </row>
+    <row r="9" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>44689</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="17">
         <v>44693</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="I9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="18"/>
+    </row>
+    <row r="10" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>44690</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="17">
         <v>44693</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="27"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="J10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+      <c r="AA10" s="18"/>
+    </row>
+    <row r="11" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>44686</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="17">
         <v>44691</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="27"/>
+      <c r="F11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="8" t="s">
+      <c r="K11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="18"/>
+    </row>
+    <row r="12" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>44689</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="17">
         <v>44690</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="27"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K12" s="9"/>
+      <c r="I12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" s="7"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+      <c r="AA12" s="18"/>
+    </row>
+    <row r="13" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>44690</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="17">
         <v>44693</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="27"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="J13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="4"/>
+      <c r="AA13" s="18"/>
+    </row>
+    <row r="14" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>44691</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="17">
         <v>44693</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="27"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="M14" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="K14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="V14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="18"/>
+    </row>
+    <row r="15" spans="1:27" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>44693</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="17">
         <v>44693</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="27"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
@@ -1119,36 +1584,117 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+      <c r="AA15" s="18"/>
+    </row>
+    <row r="16" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+      <c r="AA16" s="18"/>
+    </row>
+    <row r="17" spans="1:27" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="W17" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="21"/>
+    </row>
+    <row r="18" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1157,7 +1703,7 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E2:AA2"/>
   </mergeCells>
   <pageMargins left="0.94488188976377963" right="0.94488188976377963" top="0.94488188976377963" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>